<commit_message>
changes based on Skype meeting
</commit_message>
<xml_diff>
--- a/radtrack/util/unified_parameters.xlsx
+++ b/radtrack/util/unified_parameters.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="204">
   <si>
     <t>Parameter</t>
   </si>
@@ -402,9 +402,6 @@
     <t>Thick Beam Model</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>py_type</t>
   </si>
   <si>
@@ -519,60 +516,27 @@
     <t>$Q$</t>
   </si>
   <si>
-    <t>$\mean{x\prime}$</t>
-  </si>
-  <si>
-    <t>$\mean{x}$</t>
-  </si>
-  <si>
-    <t>$\mean{y}$</t>
-  </si>
-  <si>
-    <t>$\mean{s}$</t>
-  </si>
-  <si>
     <t>$\mean{y\prime}$</t>
   </si>
   <si>
     <t>$\mean{\gamma}$</t>
   </si>
   <si>
-    <t>$y_rms$</t>
-  </si>
-  <si>
-    <t>$x_rms$</t>
-  </si>
-  <si>
-    <t>$s_rms$</t>
-  </si>
-  <si>
-    <t>$x\prime_rms$</t>
-  </si>
-  <si>
     <t>$y\prime_rms$</t>
   </si>
   <si>
     <t>$\mean{x-x\prime}$</t>
   </si>
   <si>
-    <t>$\gamma_rms$</t>
-  </si>
-  <si>
     <t>$\nu$</t>
   </si>
   <si>
     <t>The average frequency of particle bunches in the electron synchrotron.</t>
   </si>
   <si>
-    <t>avg_current=total_charge*rf_frequency</t>
-  </si>
-  <si>
     <t>rf_frequency</t>
   </si>
   <si>
-    <t>$I_peak$</t>
-  </si>
-  <si>
     <t>rad</t>
   </si>
   <si>
@@ -588,27 +552,15 @@
     <t>avg_beta_gamma</t>
   </si>
   <si>
-    <t>avg_beta_gamma=math.sqrt(avg_gamma**2-1.)</t>
-  </si>
-  <si>
     <t>avg_beta</t>
   </si>
   <si>
-    <t>avg_beta=avg_beta_gamma/avg_gamma</t>
-  </si>
-  <si>
     <t>avg_velocity</t>
   </si>
   <si>
-    <t>$\mean{v_long}$</t>
-  </si>
-  <si>
     <t>m/s</t>
   </si>
   <si>
-    <t>avg_velocity=avg_beta*scipy.constants.c</t>
-  </si>
-  <si>
     <t>$\mean{\beta}$</t>
   </si>
   <si>
@@ -618,9 +570,6 @@
     <t>$\mean{\beta\gamma}$</t>
   </si>
   <si>
-    <t>rms_peak_current=total_charge*avg_velocity/rms_s</t>
-  </si>
-  <si>
     <t>avg_kinetic_energy</t>
   </si>
   <si>
@@ -633,7 +582,61 @@
     <t>MeV</t>
   </si>
   <si>
-    <t>avg_kinetic_energy=(avg_gamma-1.)*scipy.constants.physical_constants["electron mass energy equivalent in MeV"][0]</t>
+    <t>py_name</t>
+  </si>
+  <si>
+    <t>$x_{rms}$</t>
+  </si>
+  <si>
+    <t>$y_{rms}$</t>
+  </si>
+  <si>
+    <t>$x\prime_{rms}$</t>
+  </si>
+  <si>
+    <t>$&lt;x&gt;$</t>
+  </si>
+  <si>
+    <t>$s_{rms}$</t>
+  </si>
+  <si>
+    <t>$&lt;y&gt;$</t>
+  </si>
+  <si>
+    <t>$&lt;s&gt;$</t>
+  </si>
+  <si>
+    <t>$&lt;x\prime&gt;$</t>
+  </si>
+  <si>
+    <t>$I_{peak}$</t>
+  </si>
+  <si>
+    <t>$\mean{v_{long}}$</t>
+  </si>
+  <si>
+    <t>==total_charge*rf_frequency</t>
+  </si>
+  <si>
+    <t>==math.sqrt(avg_gamma*G19*2-1)</t>
+  </si>
+  <si>
+    <t>==avg_beta_gamma/avg_gamma</t>
+  </si>
+  <si>
+    <t>$\gamma_{rms}$</t>
+  </si>
+  <si>
+    <t>==avg_beta*scipy.constants.c</t>
+  </si>
+  <si>
+    <t>==total_charge*avg_velocity/rms_s</t>
+  </si>
+  <si>
+    <t>==(avg_gamma-1.)*physical_constants["electron mass energy equivalent in MeV"][0]</t>
+  </si>
+  <si>
+    <t>note:  physical_constants corresponds to scipy.constants.physical_constants</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1447,6 +1450,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1754,8 +1770,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1766,79 +1782,79 @@
     <col min="4" max="4" width="16.28515625" style="78" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="78" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="78" customWidth="1"/>
-    <col min="7" max="7" width="163.5703125" style="78" customWidth="1"/>
+    <col min="7" max="7" width="163.5703125" style="103" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="78"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="74" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
       <c r="D1" s="68"/>
       <c r="E1" s="68"/>
       <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="G1" s="99"/>
       <c r="H1" s="73"/>
     </row>
     <row r="2" spans="1:8" s="76" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="69" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="69" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="69" t="s">
+      <c r="D2" s="69" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="E2" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="100" t="s">
         <v>127</v>
-      </c>
-      <c r="E2" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="69" t="s">
-        <v>128</v>
       </c>
       <c r="H2" s="75"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="71">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F3" s="72">
         <v>1</v>
       </c>
-      <c r="G3" s="66" t="s">
-        <v>150</v>
+      <c r="G3" s="101" t="s">
+        <v>149</v>
       </c>
       <c r="H3" s="77"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D4" s="71">
         <v>0</v>
@@ -1849,20 +1865,20 @@
       <c r="F4" s="72">
         <v>1</v>
       </c>
-      <c r="G4" s="66" t="s">
-        <v>151</v>
+      <c r="G4" s="101" t="s">
+        <v>150</v>
       </c>
       <c r="H4" s="77"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="70" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="71">
         <v>0</v>
@@ -1873,20 +1889,20 @@
       <c r="F5" s="72">
         <v>1</v>
       </c>
-      <c r="G5" s="66" t="s">
-        <v>152</v>
+      <c r="G5" s="101" t="s">
+        <v>151</v>
       </c>
       <c r="H5" s="77"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="66" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="71">
         <v>0</v>
@@ -1897,68 +1913,68 @@
       <c r="F6" s="72">
         <v>1</v>
       </c>
-      <c r="G6" s="66" t="s">
-        <v>153</v>
+      <c r="G6" s="101" t="s">
+        <v>152</v>
       </c>
       <c r="H6" s="77"/>
     </row>
     <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="66" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="C7" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="71">
         <v>0</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F7" s="72">
         <v>1</v>
       </c>
-      <c r="G7" s="66" t="s">
-        <v>154</v>
+      <c r="G7" s="101" t="s">
+        <v>153</v>
       </c>
       <c r="H7" s="77"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="66" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C8" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="71">
         <v>0</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F8" s="72">
         <v>1</v>
       </c>
-      <c r="G8" s="66" t="s">
-        <v>155</v>
+      <c r="G8" s="101" t="s">
+        <v>154</v>
       </c>
       <c r="H8" s="77"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" s="66" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C9" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" s="71">
         <v>1000000000</v>
@@ -1967,20 +1983,20 @@
       <c r="F9" s="72">
         <v>1</v>
       </c>
-      <c r="G9" s="66" t="s">
-        <v>156</v>
+      <c r="G9" s="101" t="s">
+        <v>155</v>
       </c>
       <c r="H9" s="77"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D10" s="71">
         <v>1E-4</v>
@@ -1991,20 +2007,20 @@
       <c r="F10" s="72">
         <v>1</v>
       </c>
-      <c r="G10" s="66" t="s">
-        <v>157</v>
+      <c r="G10" s="101" t="s">
+        <v>156</v>
       </c>
       <c r="H10" s="77"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11" s="66" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="C11" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" s="71">
         <v>1E-4</v>
@@ -2015,20 +2031,20 @@
       <c r="F11" s="72">
         <v>1</v>
       </c>
-      <c r="G11" s="66" t="s">
-        <v>158</v>
+      <c r="G11" s="101" t="s">
+        <v>157</v>
       </c>
       <c r="H11" s="77"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="C12" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" s="71">
         <v>1E-4</v>
@@ -2039,116 +2055,116 @@
       <c r="F12" s="72">
         <v>1</v>
       </c>
-      <c r="G12" s="66" t="s">
-        <v>159</v>
+      <c r="G12" s="101" t="s">
+        <v>158</v>
       </c>
       <c r="H12" s="77"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="C13" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D13" s="71">
         <v>1E-4</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F13" s="72">
         <v>1</v>
       </c>
-      <c r="G13" s="66" t="s">
-        <v>160</v>
+      <c r="G13" s="101" t="s">
+        <v>159</v>
       </c>
       <c r="H13" s="77"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14" s="66" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" s="71">
         <v>1E-4</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F14" s="72">
         <v>1</v>
       </c>
-      <c r="G14" s="66" t="s">
+      <c r="G14" s="101" t="s">
         <v>99</v>
       </c>
       <c r="H14" s="77"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="66" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C15" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D15" s="71">
         <v>0</v>
       </c>
       <c r="E15" s="72" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F15" s="72">
         <v>1</v>
       </c>
-      <c r="G15" s="66" t="s">
-        <v>161</v>
+      <c r="G15" s="101" t="s">
+        <v>160</v>
       </c>
       <c r="H15" s="77"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16" s="66" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="C16" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D16" s="71">
         <v>0</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F16" s="72">
         <v>1</v>
       </c>
-      <c r="G16" s="66" t="s">
+      <c r="G16" s="101" t="s">
         <v>98</v>
       </c>
       <c r="H16" s="77"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="66" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="66" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="C17" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D17" s="71">
         <v>1E-3</v>
@@ -2157,44 +2173,44 @@
       <c r="F17" s="72">
         <v>1</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="101" t="s">
         <v>97</v>
       </c>
       <c r="H17" s="77"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="66" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B18" s="66" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C18" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D18" s="71">
         <v>1000000</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="F18" s="72">
         <v>1</v>
       </c>
-      <c r="G18" s="66" t="s">
-        <v>178</v>
+      <c r="G18" s="101" t="s">
+        <v>168</v>
       </c>
       <c r="H18" s="77"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" s="66" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="C19" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D19" s="71"/>
       <c r="E19" s="72" t="s">
@@ -2203,82 +2219,82 @@
       <c r="F19" s="72">
         <v>0</v>
       </c>
-      <c r="G19" s="66" t="s">
-        <v>179</v>
+      <c r="G19" s="101" t="s">
+        <v>196</v>
       </c>
       <c r="H19" s="77"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="66" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C20" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D20" s="71"/>
       <c r="E20" s="72"/>
       <c r="F20" s="72">
         <v>0</v>
       </c>
-      <c r="G20" s="66" t="s">
-        <v>187</v>
+      <c r="G20" s="101" t="s">
+        <v>197</v>
       </c>
       <c r="H20" s="77"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="66" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B21" s="66" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D21" s="71"/>
       <c r="E21" s="72"/>
       <c r="F21" s="72">
         <v>0</v>
       </c>
-      <c r="G21" s="66" t="s">
-        <v>189</v>
+      <c r="G21" s="101" t="s">
+        <v>198</v>
       </c>
       <c r="H21" s="77"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="66" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="B22" s="66" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C22" s="72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D22" s="71"/>
       <c r="E22" s="72" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="F22" s="72">
         <v>0</v>
       </c>
-      <c r="G22" s="66" t="s">
-        <v>193</v>
+      <c r="G22" s="101" t="s">
+        <v>200</v>
       </c>
       <c r="H22" s="77"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="67" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B23" s="67" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="C23" s="79" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D23" s="80"/>
       <c r="E23" s="79" t="s">
@@ -2287,29 +2303,29 @@
       <c r="F23" s="79">
         <v>0</v>
       </c>
-      <c r="G23" s="67" t="s">
-        <v>197</v>
+      <c r="G23" s="102" t="s">
+        <v>201</v>
       </c>
       <c r="H23" s="77"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="78" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B24" s="78" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C24" s="81" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" s="82"/>
       <c r="E24" s="81" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="F24" s="81">
         <v>0</v>
       </c>
-      <c r="G24" s="78" t="s">
+      <c r="G24" s="103" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2324,6 +2340,9 @@
       <c r="D26" s="82"/>
       <c r="E26" s="81"/>
       <c r="F26" s="81"/>
+      <c r="G26" s="103" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C27" s="81"/>

</xml_diff>

<commit_message>
renamed top-level examples directory
'examples' was misleading, so I changed the name to 'experimental'
This code was intended in part as a sandbox for testing out the RadTrack
API and in part has a place to develop tests of individual RadTrack
modules.
Some of this code should be used to develop proper tests.
Some of this code will be useful for further developing native RadTrack
features.
</commit_message>
<xml_diff>
--- a/radtrack/util/unified_parameters.xlsx
+++ b/radtrack/util/unified_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="804"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7635" tabRatio="804"/>
   </bookViews>
   <sheets>
     <sheet name="ParticleBeam" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="208">
   <si>
     <t>Parameter</t>
   </si>
@@ -516,27 +516,15 @@
     <t>$Q$</t>
   </si>
   <si>
-    <t>$\mean{y\prime}$</t>
-  </si>
-  <si>
-    <t>$\mean{\gamma}$</t>
-  </si>
-  <si>
     <t>$y\prime_rms$</t>
   </si>
   <si>
-    <t>$\mean{x-x\prime}$</t>
-  </si>
-  <si>
     <t>$\nu$</t>
   </si>
   <si>
     <t>The average frequency of particle bunches in the electron synchrotron.</t>
   </si>
   <si>
-    <t>rf_frequency</t>
-  </si>
-  <si>
     <t>rad</t>
   </si>
   <si>
@@ -573,9 +561,6 @@
     <t>avg_kinetic_energy</t>
   </si>
   <si>
-    <t>$\mean{y-y\prime}$</t>
-  </si>
-  <si>
     <t>$\mean{E}$</t>
   </si>
   <si>
@@ -615,28 +600,55 @@
     <t>$\mean{v_{long}}$</t>
   </si>
   <si>
-    <t>==total_charge*rf_frequency</t>
-  </si>
-  <si>
-    <t>==math.sqrt(avg_gamma*G19*2-1)</t>
-  </si>
-  <si>
-    <t>==avg_beta_gamma/avg_gamma</t>
-  </si>
-  <si>
     <t>$\gamma_{rms}$</t>
   </si>
   <si>
-    <t>==avg_beta*scipy.constants.c</t>
-  </si>
-  <si>
-    <t>==total_charge*avg_velocity/rms_s</t>
-  </si>
-  <si>
-    <t>==(avg_gamma-1.)*physical_constants["electron mass energy equivalent in MeV"][0]</t>
-  </si>
-  <si>
     <t>note:  physical_constants corresponds to scipy.constants.physical_constants</t>
+  </si>
+  <si>
+    <t>rep_frequency</t>
+  </si>
+  <si>
+    <t>avg_beta_gamma/avg_gamma</t>
+  </si>
+  <si>
+    <t>avg_beta*scipy.constants.c</t>
+  </si>
+  <si>
+    <t>total_charge*avg_velocity/rms_s</t>
+  </si>
+  <si>
+    <t>(avg_gamma-1.)*physical_constants["electron mass energy equivalent in MeV"][0]</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>from scipy.constants import physical_constants</t>
+  </si>
+  <si>
+    <t>import scipy</t>
+  </si>
+  <si>
+    <t>total_charge*rf_frequency   #:The average current.</t>
+  </si>
+  <si>
+    <t>math.sqrt(avg_gamma*2-1)    #:The average value of relativistic beta</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>$&lt;y\prime&gt;$</t>
+  </si>
+  <si>
+    <t>$&lt;\gamma&gt;$</t>
+  </si>
+  <si>
+    <t>$&lt;x-x\prime&gt;$</t>
+  </si>
+  <si>
+    <t>$&lt;y-y\prime&gt;$</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1405,6 +1417,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -1450,19 +1475,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1770,8 +1785,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1782,7 +1797,7 @@
     <col min="4" max="4" width="16.28515625" style="78" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="78" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" style="78" customWidth="1"/>
-    <col min="7" max="7" width="163.5703125" style="103" customWidth="1"/>
+    <col min="7" max="7" width="163.5703125" style="88" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="78"/>
   </cols>
   <sheetData>
@@ -1795,12 +1810,12 @@
       <c r="D1" s="68"/>
       <c r="E1" s="68"/>
       <c r="F1" s="68"/>
-      <c r="G1" s="99"/>
+      <c r="G1" s="84"/>
       <c r="H1" s="73"/>
     </row>
     <row r="2" spans="1:8" s="76" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="69" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B2" s="69" t="s">
         <v>131</v>
@@ -1817,89 +1832,63 @@
       <c r="F2" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="100" t="s">
+      <c r="G2" s="85" t="s">
         <v>127</v>
       </c>
       <c r="H2" s="75"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="81" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="82"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="88" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="81" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="82"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="88" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B5" s="66" t="s">
         <v>162</v>
-      </c>
-      <c r="C3" s="72" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="71">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="E3" s="72" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" s="72">
-        <v>1</v>
-      </c>
-      <c r="G3" s="101" t="s">
-        <v>149</v>
-      </c>
-      <c r="H3" s="77"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="66" t="s">
-        <v>189</v>
-      </c>
-      <c r="C4" s="72" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="71">
-        <v>0</v>
-      </c>
-      <c r="E4" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="72">
-        <v>1</v>
-      </c>
-      <c r="G4" s="101" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" s="77"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="70" t="s">
-        <v>191</v>
       </c>
       <c r="C5" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D5" s="71">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="E5" s="72" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="F5" s="72">
         <v>1</v>
       </c>
-      <c r="G5" s="101" t="s">
-        <v>151</v>
+      <c r="G5" s="86" t="s">
+        <v>149</v>
       </c>
       <c r="H5" s="77"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="66" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B6" s="66" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C6" s="72" t="s">
         <v>130</v>
@@ -1913,17 +1902,17 @@
       <c r="F6" s="72">
         <v>1</v>
       </c>
-      <c r="G6" s="101" t="s">
-        <v>152</v>
+      <c r="G6" s="86" t="s">
+        <v>150</v>
       </c>
       <c r="H6" s="77"/>
     </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="66" t="s">
-        <v>193</v>
+        <v>134</v>
+      </c>
+      <c r="B7" s="70" t="s">
+        <v>186</v>
       </c>
       <c r="C7" s="72" t="s">
         <v>130</v>
@@ -1932,22 +1921,22 @@
         <v>0</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>170</v>
+        <v>2</v>
       </c>
       <c r="F7" s="72">
         <v>1</v>
       </c>
-      <c r="G7" s="101" t="s">
-        <v>153</v>
+      <c r="G7" s="86" t="s">
+        <v>151</v>
       </c>
       <c r="H7" s="77"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B8" s="66" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="C8" s="72" t="s">
         <v>130</v>
@@ -1956,92 +1945,92 @@
         <v>0</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>170</v>
+        <v>2</v>
       </c>
       <c r="F8" s="72">
         <v>1</v>
       </c>
-      <c r="G8" s="101" t="s">
-        <v>154</v>
+      <c r="G8" s="86" t="s">
+        <v>152</v>
       </c>
       <c r="H8" s="77"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B9" s="66" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="C9" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D9" s="71">
-        <v>1000000000</v>
-      </c>
-      <c r="E9" s="72"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="72" t="s">
+        <v>166</v>
+      </c>
       <c r="F9" s="72">
         <v>1</v>
       </c>
-      <c r="G9" s="101" t="s">
-        <v>155</v>
+      <c r="G9" s="86" t="s">
+        <v>153</v>
       </c>
       <c r="H9" s="77"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="66" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B10" s="66" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="C10" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D10" s="71">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>2</v>
+        <v>166</v>
       </c>
       <c r="F10" s="72">
         <v>1</v>
       </c>
-      <c r="G10" s="101" t="s">
-        <v>156</v>
+      <c r="G10" s="86" t="s">
+        <v>154</v>
       </c>
       <c r="H10" s="77"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="66" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B11" s="66" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="C11" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D11" s="71">
-        <v>1E-4</v>
-      </c>
-      <c r="E11" s="72" t="s">
-        <v>2</v>
-      </c>
+        <v>1000000000</v>
+      </c>
+      <c r="E11" s="72"/>
       <c r="F11" s="72">
         <v>1</v>
       </c>
-      <c r="G11" s="101" t="s">
-        <v>157</v>
+      <c r="G11" s="86" t="s">
+        <v>155</v>
       </c>
       <c r="H11" s="77"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B12" s="66" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C12" s="72" t="s">
         <v>130</v>
@@ -2055,17 +2044,17 @@
       <c r="F12" s="72">
         <v>1</v>
       </c>
-      <c r="G12" s="101" t="s">
-        <v>158</v>
+      <c r="G12" s="86" t="s">
+        <v>156</v>
       </c>
       <c r="H12" s="77"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="66" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B13" s="66" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C13" s="72" t="s">
         <v>130</v>
@@ -2074,22 +2063,22 @@
         <v>1E-4</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>170</v>
+        <v>2</v>
       </c>
       <c r="F13" s="72">
         <v>1</v>
       </c>
-      <c r="G13" s="101" t="s">
-        <v>159</v>
+      <c r="G13" s="86" t="s">
+        <v>157</v>
       </c>
       <c r="H13" s="77"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="66" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B14" s="66" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>130</v>
@@ -2098,250 +2087,283 @@
         <v>1E-4</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>170</v>
+        <v>2</v>
       </c>
       <c r="F14" s="72">
         <v>1</v>
       </c>
-      <c r="G14" s="101" t="s">
-        <v>99</v>
+      <c r="G14" s="86" t="s">
+        <v>158</v>
       </c>
       <c r="H14" s="77"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="66" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B15" s="66" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="C15" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D15" s="71">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="E15" s="72" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F15" s="72">
         <v>1</v>
       </c>
-      <c r="G15" s="101" t="s">
-        <v>160</v>
+      <c r="G15" s="86" t="s">
+        <v>159</v>
       </c>
       <c r="H15" s="77"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="66" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B16" s="66" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C16" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D16" s="71">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="E16" s="72" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F16" s="72">
         <v>1</v>
       </c>
-      <c r="G16" s="101" t="s">
-        <v>98</v>
+      <c r="G16" s="86" t="s">
+        <v>99</v>
       </c>
       <c r="H16" s="77"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="66" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B17" s="66" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C17" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D17" s="71">
-        <v>1E-3</v>
-      </c>
-      <c r="E17" s="72"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>167</v>
+      </c>
       <c r="F17" s="72">
         <v>1</v>
       </c>
-      <c r="G17" s="101" t="s">
-        <v>97</v>
+      <c r="G17" s="86" t="s">
+        <v>160</v>
       </c>
       <c r="H17" s="77"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="66" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="B18" s="66" t="s">
-        <v>167</v>
+        <v>207</v>
       </c>
       <c r="C18" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D18" s="71">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E18" s="72" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F18" s="72">
         <v>1</v>
       </c>
-      <c r="G18" s="101" t="s">
-        <v>168</v>
+      <c r="G18" s="86" t="s">
+        <v>98</v>
       </c>
       <c r="H18" s="77"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="66" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B19" s="66" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="C19" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="72" t="s">
-        <v>39</v>
-      </c>
+      <c r="D19" s="71">
+        <v>1E-3</v>
+      </c>
+      <c r="E19" s="72"/>
       <c r="F19" s="72">
-        <v>0</v>
-      </c>
-      <c r="G19" s="101" t="s">
-        <v>196</v>
+        <v>1</v>
+      </c>
+      <c r="G19" s="86" t="s">
+        <v>97</v>
       </c>
       <c r="H19" s="77"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="66" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C20" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="71"/>
-      <c r="E20" s="72"/>
+      <c r="D20" s="71">
+        <v>1000000</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>168</v>
+      </c>
       <c r="F20" s="72">
-        <v>0</v>
-      </c>
-      <c r="G20" s="101" t="s">
-        <v>197</v>
+        <v>1</v>
+      </c>
+      <c r="G20" s="86" t="s">
+        <v>165</v>
       </c>
       <c r="H20" s="77"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="66" t="s">
         <v>175</v>
-      </c>
-      <c r="B21" s="66" t="s">
-        <v>178</v>
       </c>
       <c r="C21" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D21" s="71"/>
-      <c r="E21" s="72"/>
+      <c r="E21" s="72" t="s">
+        <v>39</v>
+      </c>
       <c r="F21" s="72">
         <v>0</v>
       </c>
-      <c r="G21" s="101" t="s">
-        <v>198</v>
+      <c r="G21" s="104" t="s">
+        <v>201</v>
       </c>
       <c r="H21" s="77"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="66" t="s">
         <v>176</v>
-      </c>
-      <c r="B22" s="66" t="s">
-        <v>195</v>
       </c>
       <c r="C22" s="72" t="s">
         <v>130</v>
       </c>
       <c r="D22" s="71"/>
-      <c r="E22" s="72" t="s">
-        <v>177</v>
-      </c>
+      <c r="E22" s="72"/>
       <c r="F22" s="72">
         <v>0</v>
       </c>
-      <c r="G22" s="101" t="s">
-        <v>200</v>
+      <c r="G22" s="86" t="s">
+        <v>202</v>
       </c>
       <c r="H22" s="77"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="67" t="s">
+      <c r="A23" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="71"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72">
+        <v>0</v>
+      </c>
+      <c r="G23" s="86" t="s">
+        <v>194</v>
+      </c>
+      <c r="H23" s="77"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="66" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="71"/>
+      <c r="E24" s="72" t="s">
         <v>173</v>
       </c>
-      <c r="B23" s="67" t="s">
-        <v>194</v>
-      </c>
-      <c r="C23" s="79" t="s">
+      <c r="F24" s="72">
+        <v>0</v>
+      </c>
+      <c r="G24" s="86" t="s">
+        <v>195</v>
+      </c>
+      <c r="H24" s="77"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="67" t="s">
+        <v>169</v>
+      </c>
+      <c r="B25" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="80"/>
-      <c r="E23" s="79" t="s">
+      <c r="D25" s="80"/>
+      <c r="E25" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="79">
+      <c r="F25" s="79">
         <v>0</v>
       </c>
-      <c r="G23" s="102" t="s">
-        <v>201</v>
-      </c>
-      <c r="H23" s="77"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="78" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24" s="78" t="s">
-        <v>183</v>
-      </c>
-      <c r="C24" s="81" t="s">
+      <c r="G25" s="87" t="s">
+        <v>196</v>
+      </c>
+      <c r="H25" s="77"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="C26" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="D24" s="82"/>
-      <c r="E24" s="81" t="s">
-        <v>184</v>
-      </c>
-      <c r="F24" s="81">
+      <c r="D26" s="82"/>
+      <c r="E26" s="81" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" s="81">
         <v>0</v>
       </c>
-      <c r="G24" s="103" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="81"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="81"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="103" t="s">
-        <v>203</v>
+      <c r="G26" s="88" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2363,10 +2385,15 @@
       <c r="F29" s="81"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="81"/>
+      <c r="C30" s="81" t="s">
+        <v>203</v>
+      </c>
       <c r="D30" s="82"/>
       <c r="E30" s="81"/>
       <c r="F30" s="81"/>
+      <c r="G30" s="88" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="81"/>
@@ -2639,7 +2666,7 @@
       <c r="F1" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="89" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2660,7 +2687,7 @@
       <c r="F2" s="44">
         <v>1</v>
       </c>
-      <c r="G2" s="85"/>
+      <c r="G2" s="90"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2679,7 +2706,7 @@
       <c r="F3" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="85"/>
+      <c r="G3" s="90"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -2700,7 +2727,7 @@
       <c r="F4" s="46">
         <v>1.85</v>
       </c>
-      <c r="G4" s="85"/>
+      <c r="G4" s="90"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -2721,7 +2748,7 @@
       <c r="F5" s="46">
         <v>0.1</v>
       </c>
-      <c r="G5" s="85"/>
+      <c r="G5" s="90"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
@@ -2740,7 +2767,7 @@
       <c r="F6" s="48">
         <v>30</v>
       </c>
-      <c r="G6" s="85"/>
+      <c r="G6" s="90"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="49">
@@ -2921,7 +2948,7 @@
       <c r="C2" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="91" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2935,7 +2962,7 @@
       <c r="C3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="87"/>
+      <c r="D3" s="92"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
@@ -2947,7 +2974,7 @@
       <c r="C4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="87"/>
+      <c r="D4" s="92"/>
     </row>
     <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
@@ -2959,7 +2986,7 @@
       <c r="C5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="87"/>
+      <c r="D5" s="92"/>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
@@ -2971,7 +2998,7 @@
       <c r="C6" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="88"/>
+      <c r="D6" s="93"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2984,7 +3011,7 @@
       <c r="C8" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="86" t="s">
+      <c r="D8" s="91" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2998,7 +3025,7 @@
       <c r="C9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="89"/>
+      <c r="D9" s="94"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
@@ -3010,7 +3037,7 @@
       <c r="C10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="89"/>
+      <c r="D10" s="94"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
@@ -3022,7 +3049,7 @@
       <c r="C11" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="89"/>
+      <c r="D11" s="94"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
@@ -3034,7 +3061,7 @@
       <c r="C12" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="90"/>
+      <c r="D12" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3089,7 +3116,7 @@
       <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="96" t="s">
         <v>53</v>
       </c>
       <c r="E2" s="60">
@@ -3098,7 +3125,7 @@
       <c r="F2" s="61">
         <v>1</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="89" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3110,14 +3137,14 @@
       <c r="C3" s="10">
         <v>100</v>
       </c>
-      <c r="D3" s="92"/>
+      <c r="D3" s="97"/>
       <c r="E3" s="49">
         <v>100</v>
       </c>
       <c r="F3" s="50">
         <v>100</v>
       </c>
-      <c r="G3" s="97"/>
+      <c r="G3" s="102"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -3127,14 +3154,14 @@
       <c r="C4" s="10">
         <v>100</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="49">
         <v>100</v>
       </c>
       <c r="F4" s="50">
         <v>100</v>
       </c>
-      <c r="G4" s="97"/>
+      <c r="G4" s="102"/>
     </row>
     <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -3146,14 +3173,14 @@
       <c r="C5" s="10">
         <v>20</v>
       </c>
-      <c r="D5" s="92"/>
+      <c r="D5" s="97"/>
       <c r="E5" s="49">
         <v>20</v>
       </c>
       <c r="F5" s="50">
         <v>20</v>
       </c>
-      <c r="G5" s="97"/>
+      <c r="G5" s="102"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -3165,10 +3192,10 @@
       <c r="C6" s="6">
         <v>2774</v>
       </c>
-      <c r="D6" s="92"/>
+      <c r="D6" s="97"/>
       <c r="E6" s="49"/>
       <c r="F6" s="50"/>
-      <c r="G6" s="97"/>
+      <c r="G6" s="102"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -3180,10 +3207,10 @@
       <c r="C7" s="6">
         <v>2774</v>
       </c>
-      <c r="D7" s="92"/>
+      <c r="D7" s="97"/>
       <c r="E7" s="49"/>
       <c r="F7" s="50"/>
-      <c r="G7" s="97"/>
+      <c r="G7" s="102"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -3195,14 +3222,14 @@
       <c r="C8" s="2">
         <v>-1E-3</v>
       </c>
-      <c r="D8" s="92"/>
+      <c r="D8" s="97"/>
       <c r="E8" s="56">
         <v>-1E-4</v>
       </c>
       <c r="F8" s="57">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="G8" s="97"/>
+      <c r="G8" s="102"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -3214,14 +3241,14 @@
       <c r="C9" s="2">
         <v>1E-3</v>
       </c>
-      <c r="D9" s="92"/>
+      <c r="D9" s="97"/>
       <c r="E9" s="56">
         <v>1E-4</v>
       </c>
       <c r="F9" s="57">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G9" s="97"/>
+      <c r="G9" s="102"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -3233,14 +3260,14 @@
       <c r="C10" s="2">
         <v>-1E-3</v>
       </c>
-      <c r="D10" s="92"/>
+      <c r="D10" s="97"/>
       <c r="E10" s="56">
         <v>-1E-4</v>
       </c>
       <c r="F10" s="57">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="G10" s="97"/>
+      <c r="G10" s="102"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
@@ -3252,14 +3279,14 @@
       <c r="C11" s="2">
         <v>1E-3</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="98"/>
       <c r="E11" s="58">
         <v>1E-4</v>
       </c>
       <c r="F11" s="59">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G11" s="98"/>
+      <c r="G11" s="103"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="32">
@@ -3274,7 +3301,7 @@
       <c r="C13" s="13">
         <v>10000</v>
       </c>
-      <c r="D13" s="94" t="s">
+      <c r="D13" s="99" t="s">
         <v>54</v>
       </c>
       <c r="E13" s="54">
@@ -3283,7 +3310,7 @@
       <c r="F13" s="55">
         <v>1</v>
       </c>
-      <c r="G13" s="84" t="s">
+      <c r="G13" s="89" t="s">
         <v>91</v>
       </c>
     </row>
@@ -3295,14 +3322,14 @@
       <c r="C14" s="10">
         <v>1</v>
       </c>
-      <c r="D14" s="95"/>
+      <c r="D14" s="100"/>
       <c r="E14" s="49">
         <v>100</v>
       </c>
       <c r="F14" s="50">
         <v>100</v>
       </c>
-      <c r="G14" s="97"/>
+      <c r="G14" s="102"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -3312,14 +3339,14 @@
       <c r="C15" s="10">
         <v>1</v>
       </c>
-      <c r="D15" s="95"/>
+      <c r="D15" s="100"/>
       <c r="E15" s="49">
         <v>100</v>
       </c>
       <c r="F15" s="50">
         <v>100</v>
       </c>
-      <c r="G15" s="97"/>
+      <c r="G15" s="102"/>
     </row>
     <row r="16" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -3331,14 +3358,14 @@
       <c r="C16" s="10">
         <v>20</v>
       </c>
-      <c r="D16" s="95"/>
+      <c r="D16" s="100"/>
       <c r="E16" s="49">
         <v>20</v>
       </c>
       <c r="F16" s="50">
         <v>20</v>
       </c>
-      <c r="G16" s="97"/>
+      <c r="G16" s="102"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -3350,10 +3377,10 @@
       <c r="C17" s="6">
         <v>20</v>
       </c>
-      <c r="D17" s="95"/>
+      <c r="D17" s="100"/>
       <c r="E17" s="49"/>
       <c r="F17" s="50"/>
-      <c r="G17" s="97"/>
+      <c r="G17" s="102"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -3365,10 +3392,10 @@
       <c r="C18" s="6">
         <v>3000</v>
       </c>
-      <c r="D18" s="95"/>
+      <c r="D18" s="100"/>
       <c r="E18" s="49"/>
       <c r="F18" s="50"/>
-      <c r="G18" s="97"/>
+      <c r="G18" s="102"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -3381,14 +3408,14 @@
         <f>-C12</f>
         <v>-1.1999999999999999E-6</v>
       </c>
-      <c r="D19" s="95"/>
+      <c r="D19" s="100"/>
       <c r="E19" s="56">
         <v>-1E-4</v>
       </c>
       <c r="F19" s="57">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="G19" s="97"/>
+      <c r="G19" s="102"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -3401,14 +3428,14 @@
         <f>C12</f>
         <v>1.1999999999999999E-6</v>
       </c>
-      <c r="D20" s="95"/>
+      <c r="D20" s="100"/>
       <c r="E20" s="56">
         <v>1E-4</v>
       </c>
       <c r="F20" s="57">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G20" s="97"/>
+      <c r="G20" s="102"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -3421,14 +3448,14 @@
         <f>-C$12</f>
         <v>-1.1999999999999999E-6</v>
       </c>
-      <c r="D21" s="95"/>
+      <c r="D21" s="100"/>
       <c r="E21" s="56">
         <v>-1E-4</v>
       </c>
       <c r="F21" s="57">
         <v>-5.0000000000000001E-3</v>
       </c>
-      <c r="G21" s="97"/>
+      <c r="G21" s="102"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -3441,14 +3468,14 @@
         <f>C$12</f>
         <v>1.1999999999999999E-6</v>
       </c>
-      <c r="D22" s="96"/>
+      <c r="D22" s="101"/>
       <c r="E22" s="58">
         <v>1E-4</v>
       </c>
       <c r="F22" s="59">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G22" s="98"/>
+      <c r="G22" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>